<commit_message>
Juan Carlos Rojas Buitrago
Alimentar HU en Jira, se deja enlace correspondiente y se deja en Daily Scrum la actividad
</commit_message>
<xml_diff>
--- a/Sprint 1/Ceremonias/Sprint planning/Daily Scrum.xlsx
+++ b/Sprint 1/Ceremonias/Sprint planning/Daily Scrum.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inde\Documents\GitHub\mcds-2238280-proyecto\Sprint 1\Ceremonias\Sprint planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F05D6CB-EEEC-4015-B743-EE8690E4CF93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6958AD92-C8A8-45D1-B9EB-708B8D44DC08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>¿Qué hice ayer?</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Crear repositorio y subcarpetas</t>
+  </si>
+  <si>
+    <t>Creación repositorio</t>
+  </si>
+  <si>
+    <t>Diagrama de base de datos</t>
+  </si>
+  <si>
+    <t>Alimentación repositorio</t>
+  </si>
+  <si>
+    <t>Alimentación HU en Jira</t>
   </si>
 </sst>
 </file>
@@ -382,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -393,8 +405,8 @@
     <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -456,6 +468,41 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <v>44316</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44318</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>